<commit_message>
Menambahkan Project baru untuk menampilkan "10 Penderita Berdasarkan Usia" 5212100084 - KPPL D
</commit_message>
<xml_diff>
--- a/PembagianTugas.xlsx
+++ b/PembagianTugas.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Data Chart dan  Map" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -196,8 +196,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +320,31 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,13 +354,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -356,25 +375,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +394,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -427,6 +437,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -435,11 +446,13 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -463,6 +476,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AQ$23:$AQ$32</c:f>
@@ -564,6 +578,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AQ$23:$AQ$32</c:f>
@@ -665,6 +680,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AQ$23:$AQ$32</c:f>
@@ -766,6 +782,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AQ$23:$AQ$32</c:f>
@@ -867,6 +884,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AQ$23:$AQ$32</c:f>
@@ -968,6 +986,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AQ$23:$AQ$32</c:f>
@@ -1046,19 +1065,29 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="87336064"/>
-        <c:axId val="87337600"/>
+        <c:axId val="38827520"/>
+        <c:axId val="38829056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87336064"/>
+        <c:axId val="38827520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1093,17 +1122,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87337600"/>
+        <c:crossAx val="38829056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87337600"/>
+        <c:axId val="38829056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1121,6 +1152,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1149,7 +1181,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87336064"/>
+        <c:crossAx val="38827520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1164,6 +1196,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1194,6 +1227,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1230,7 +1264,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1259,6 +1303,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1267,11 +1312,13 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1295,6 +1342,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AY$23:$AY$32</c:f>
@@ -1396,6 +1444,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AY$23:$AY$32</c:f>
@@ -1474,20 +1523,29 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="86994944"/>
-        <c:axId val="86996480"/>
+        <c:axId val="38875904"/>
+        <c:axId val="38877440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86994944"/>
+        <c:axId val="38875904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1522,17 +1580,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86996480"/>
+        <c:crossAx val="38877440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86996480"/>
+        <c:axId val="38877440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1550,6 +1610,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1578,7 +1639,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86994944"/>
+        <c:crossAx val="38875904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1593,6 +1654,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1623,6 +1685,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1659,7 +1722,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1692,6 +1765,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1700,11 +1774,13 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1728,6 +1804,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AQ$36:$AQ$45</c:f>
@@ -1829,6 +1906,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AQ$36:$AQ$45</c:f>
@@ -1930,6 +2008,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AQ$36:$AQ$45</c:f>
@@ -2031,6 +2110,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AQ$36:$AQ$45</c:f>
@@ -2132,6 +2212,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AQ$36:$AQ$45</c:f>
@@ -2233,6 +2314,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Data Chart dan  Map'!$AQ$36:$AQ$45</c:f>
@@ -2311,19 +2393,29 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="87543168"/>
-        <c:axId val="87553152"/>
+        <c:axId val="38957824"/>
+        <c:axId val="38959360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87543168"/>
+        <c:axId val="38957824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2358,17 +2450,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87553152"/>
+        <c:crossAx val="38959360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87553152"/>
+        <c:axId val="38959360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2386,6 +2480,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2414,7 +2509,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87543168"/>
+        <c:crossAx val="38957824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2429,6 +2524,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2459,6 +2555,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2495,7 +2592,17 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2529,6 +2636,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2537,11 +2645,13 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2565,6 +2675,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>[1]Sheet1!$D$33:$D$43</c:f>
@@ -2672,6 +2783,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>[1]Sheet1!$D$33:$D$43</c:f>
@@ -2779,6 +2891,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>[1]Sheet1!$D$33:$D$43</c:f>
@@ -2863,20 +2976,29 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="87677184"/>
-        <c:axId val="87556096"/>
+        <c:axId val="39131776"/>
+        <c:axId val="39149952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87677184"/>
+        <c:axId val="39131776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2911,17 +3033,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87556096"/>
+        <c:crossAx val="39149952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87556096"/>
+        <c:axId val="39149952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2939,6 +3063,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2967,7 +3092,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87677184"/>
+        <c:crossAx val="39131776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2982,6 +3107,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3012,6 +3138,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3048,7 +3175,17 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3085,6 +3222,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3093,10 +3231,12 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -3213,20 +3353,31 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="87584768"/>
-        <c:axId val="87586304"/>
+        <c:smooth val="0"/>
+        <c:axId val="39170816"/>
+        <c:axId val="39172352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87584768"/>
+        <c:axId val="39170816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -3261,17 +3412,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87586304"/>
+        <c:crossAx val="39172352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87586304"/>
+        <c:axId val="39172352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -3289,6 +3442,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -3317,7 +3471,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87584768"/>
+        <c:crossAx val="39170816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3331,6 +3485,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -6197,8 +6352,8 @@
       <xdr:rowOff>83343</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>338137</xdr:colOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>371754</xdr:colOff>
       <xdr:row>79</xdr:row>
       <xdr:rowOff>16668</xdr:rowOff>
     </xdr:to>
@@ -7847,7 +8002,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -8284,26 +8439,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:BC85"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB5" sqref="AB5:AC5"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AV16" sqref="AV16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="43" width="3.7109375" customWidth="1"/>
-    <col min="44" max="44" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="28" width="3.7109375" customWidth="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="43" width="3.7109375" customWidth="1"/>
+    <col min="44" max="44" width="5.85546875" customWidth="1"/>
     <col min="45" max="45" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="3.7109375" customWidth="1"/>
+    <col min="46" max="46" width="5.7109375" customWidth="1"/>
     <col min="47" max="47" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="3.42578125" bestFit="1" customWidth="1"/>
@@ -8311,193 +8468,193 @@
     <col min="52" max="55" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:55">
-      <c r="D4" s="37" t="s">
+    <row r="4" spans="3:55" x14ac:dyDescent="0.25">
+      <c r="D4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37" t="s">
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37" t="s">
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="38" t="s">
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="33" t="s">
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
-      <c r="X4" s="35" t="s">
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="35" t="s">
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="24" t="s">
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="AG4" s="24"/>
-      <c r="AH4" s="24"/>
-      <c r="AI4" s="24"/>
-      <c r="AJ4" s="24" t="s">
+      <c r="AG4" s="27"/>
+      <c r="AH4" s="27"/>
+      <c r="AI4" s="27"/>
+      <c r="AJ4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AK4" s="24"/>
-      <c r="AL4" s="24"/>
-      <c r="AM4" s="24"/>
-      <c r="AN4" s="26" t="s">
+      <c r="AK4" s="27"/>
+      <c r="AL4" s="27"/>
+      <c r="AM4" s="27"/>
+      <c r="AN4" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="AO4" s="26"/>
-      <c r="AP4" s="26"/>
-      <c r="AQ4" s="26"/>
-      <c r="AR4" s="26" t="s">
+      <c r="AO4" s="28"/>
+      <c r="AP4" s="28"/>
+      <c r="AQ4" s="28"/>
+      <c r="AR4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="AS4" s="26"/>
-      <c r="AT4" s="26"/>
-      <c r="AU4" s="26"/>
-      <c r="AV4" s="26" t="s">
+      <c r="AS4" s="28"/>
+      <c r="AT4" s="28"/>
+      <c r="AU4" s="28"/>
+      <c r="AV4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="AW4" s="26"/>
-      <c r="AX4" s="26"/>
-      <c r="AY4" s="26"/>
-      <c r="AZ4" s="36" t="s">
+      <c r="AW4" s="28"/>
+      <c r="AX4" s="28"/>
+      <c r="AY4" s="28"/>
+      <c r="AZ4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="BA4" s="36"/>
-      <c r="BB4" s="36"/>
-      <c r="BC4" s="36"/>
+      <c r="BA4" s="26"/>
+      <c r="BB4" s="26"/>
+      <c r="BC4" s="26"/>
     </row>
-    <row r="5" spans="3:55">
-      <c r="D5" s="37" t="s">
+    <row r="5" spans="3:55" x14ac:dyDescent="0.25">
+      <c r="D5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37" t="s">
+      <c r="G5" s="23"/>
+      <c r="H5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37" t="s">
+      <c r="I5" s="23"/>
+      <c r="J5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37" t="s">
+      <c r="K5" s="23"/>
+      <c r="L5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37" t="s">
+      <c r="M5" s="23"/>
+      <c r="N5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="37"/>
-      <c r="P5" s="38" t="s">
+      <c r="O5" s="23"/>
+      <c r="P5" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38" t="s">
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="S5" s="38"/>
-      <c r="T5" s="33" t="s">
+      <c r="S5" s="24"/>
+      <c r="T5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="U5" s="33"/>
-      <c r="V5" s="33" t="s">
+      <c r="U5" s="25"/>
+      <c r="V5" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="W5" s="33"/>
-      <c r="X5" s="35" t="s">
+      <c r="W5" s="25"/>
+      <c r="X5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="35" t="s">
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="AA5" s="35"/>
-      <c r="AB5" s="35" t="s">
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="AC5" s="35"/>
-      <c r="AD5" s="35" t="s">
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="AE5" s="35"/>
-      <c r="AF5" s="24" t="s">
+      <c r="AE5" s="22"/>
+      <c r="AF5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="AG5" s="24"/>
-      <c r="AH5" s="24" t="s">
+      <c r="AG5" s="27"/>
+      <c r="AH5" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="AI5" s="24"/>
-      <c r="AJ5" s="24" t="s">
+      <c r="AI5" s="27"/>
+      <c r="AJ5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="AK5" s="24"/>
-      <c r="AL5" s="24" t="s">
+      <c r="AK5" s="27"/>
+      <c r="AL5" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="AM5" s="24"/>
-      <c r="AN5" s="26" t="s">
+      <c r="AM5" s="27"/>
+      <c r="AN5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="AO5" s="26"/>
-      <c r="AP5" s="26" t="s">
+      <c r="AO5" s="28"/>
+      <c r="AP5" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AQ5" s="26"/>
-      <c r="AR5" s="26" t="s">
+      <c r="AQ5" s="28"/>
+      <c r="AR5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="AS5" s="26"/>
-      <c r="AT5" s="26" t="s">
+      <c r="AS5" s="28"/>
+      <c r="AT5" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AU5" s="26"/>
-      <c r="AV5" s="26" t="s">
+      <c r="AU5" s="28"/>
+      <c r="AV5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="AW5" s="26"/>
-      <c r="AX5" s="26" t="s">
+      <c r="AW5" s="28"/>
+      <c r="AX5" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AY5" s="26"/>
-      <c r="AZ5" s="36" t="s">
+      <c r="AY5" s="28"/>
+      <c r="AZ5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="BA5" s="36"/>
-      <c r="BB5" s="36" t="s">
+      <c r="BA5" s="26"/>
+      <c r="BB5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="BC5" s="36"/>
+      <c r="BC5" s="26"/>
     </row>
-    <row r="6" spans="3:55">
+    <row r="6" spans="3:55" x14ac:dyDescent="0.25">
       <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
@@ -8655,7 +8812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="3:55">
+    <row r="7" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>17</v>
       </c>
@@ -8820,7 +8977,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="3:55">
+    <row r="8" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>18</v>
       </c>
@@ -8985,7 +9142,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="3:55">
+    <row r="9" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>19</v>
       </c>
@@ -9150,7 +9307,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="3:55">
+    <row r="10" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>20</v>
       </c>
@@ -9315,7 +9472,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="3:55">
+    <row r="11" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>21</v>
       </c>
@@ -9480,7 +9637,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="3:55">
+    <row r="12" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>22</v>
       </c>
@@ -9645,7 +9802,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="3:55">
+    <row r="13" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>23</v>
       </c>
@@ -9810,7 +9967,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="3:55">
+    <row r="14" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>24</v>
       </c>
@@ -9975,7 +10132,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="3:55">
+    <row r="15" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>25</v>
       </c>
@@ -10140,7 +10297,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="3:55">
+    <row r="16" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>26</v>
       </c>
@@ -10305,7 +10462,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="3:55">
+    <row r="17" spans="3:55" x14ac:dyDescent="0.25">
       <c r="AZ17" s="2">
         <f>SUM(AZ7:AZ16)</f>
         <v>548</v>
@@ -10323,7 +10480,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="19" spans="3:55">
+    <row r="19" spans="3:55" x14ac:dyDescent="0.25">
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -10373,43 +10530,43 @@
       <c r="AX19" s="2"/>
       <c r="AY19" s="2"/>
     </row>
-    <row r="20" spans="3:55">
-      <c r="D20" s="37" t="s">
+    <row r="20" spans="3:55" x14ac:dyDescent="0.25">
+      <c r="D20" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="38" t="s">
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="32" t="s">
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="34" t="s">
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="35"/>
-      <c r="S20" s="35"/>
-      <c r="T20" s="23" t="s">
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
-      <c r="X20" s="25" t="s">
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="Y20" s="26"/>
-      <c r="Z20" s="26"/>
-      <c r="AA20" s="26"/>
+      <c r="Y20" s="28"/>
+      <c r="Z20" s="28"/>
+      <c r="AA20" s="28"/>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
       <c r="AP20" s="2"/>
@@ -10423,81 +10580,81 @@
       <c r="AX20" s="2"/>
       <c r="AY20" s="2"/>
     </row>
-    <row r="21" spans="3:55">
-      <c r="D21" s="37" t="s">
+    <row r="21" spans="3:55" x14ac:dyDescent="0.25">
+      <c r="D21" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37" t="s">
+      <c r="E21" s="23"/>
+      <c r="F21" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="37"/>
-      <c r="H21" s="38" t="s">
+      <c r="G21" s="23"/>
+      <c r="H21" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38" t="s">
+      <c r="I21" s="24"/>
+      <c r="J21" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="38"/>
-      <c r="L21" s="33" t="s">
+      <c r="K21" s="24"/>
+      <c r="L21" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33" t="s">
+      <c r="M21" s="25"/>
+      <c r="N21" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="O21" s="33"/>
-      <c r="P21" s="35" t="s">
+      <c r="O21" s="25"/>
+      <c r="P21" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35" t="s">
+      <c r="Q21" s="22"/>
+      <c r="R21" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="S21" s="35"/>
-      <c r="T21" s="24" t="s">
+      <c r="S21" s="22"/>
+      <c r="T21" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="U21" s="24"/>
-      <c r="V21" s="24" t="s">
+      <c r="U21" s="27"/>
+      <c r="V21" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="W21" s="24"/>
-      <c r="X21" s="26" t="s">
+      <c r="W21" s="27"/>
+      <c r="X21" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="26" t="s">
+      <c r="Y21" s="28"/>
+      <c r="Z21" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AA21" s="26"/>
+      <c r="AA21" s="28"/>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
-      <c r="AD21" s="27" t="s">
+      <c r="AD21" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="AE21" s="27"/>
-      <c r="AF21" s="28" t="s">
+      <c r="AE21" s="34"/>
+      <c r="AF21" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="AG21" s="28"/>
-      <c r="AH21" s="29" t="s">
+      <c r="AG21" s="35"/>
+      <c r="AH21" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="AI21" s="29"/>
-      <c r="AJ21" s="30" t="s">
+      <c r="AI21" s="36"/>
+      <c r="AJ21" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="AK21" s="30"/>
-      <c r="AL21" s="31" t="s">
+      <c r="AK21" s="37"/>
+      <c r="AL21" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="AM21" s="31"/>
-      <c r="AN21" s="22" t="s">
+      <c r="AM21" s="38"/>
+      <c r="AN21" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="AO21" s="22"/>
+      <c r="AO21" s="31"/>
       <c r="AP21" s="2"/>
       <c r="AQ21" s="2"/>
       <c r="AR21" s="2"/>
@@ -10509,7 +10666,7 @@
       <c r="AX21" s="2"/>
       <c r="AY21" s="2"/>
     </row>
-    <row r="22" spans="3:55">
+    <row r="22" spans="3:55" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
         <v>15</v>
       </c>
@@ -10648,7 +10805,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="3:55">
+    <row r="23" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>17</v>
       </c>
@@ -10841,7 +10998,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="3:55">
+    <row r="24" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>18</v>
       </c>
@@ -10998,27 +11155,27 @@
         <v>18</v>
       </c>
       <c r="AR24" s="2">
-        <f t="shared" ref="AR24:AR32" si="45">AD24+AE24</f>
+        <f>AD24+AE24</f>
         <v>61</v>
       </c>
       <c r="AS24" s="2">
-        <f t="shared" ref="AS24:AS32" si="46">AE24+AF24</f>
+        <f t="shared" ref="AS24:AS32" si="45">AE24+AF24</f>
         <v>55</v>
       </c>
       <c r="AT24" s="2">
-        <f t="shared" ref="AT24:AT32" si="47">AF24+AG24</f>
+        <f t="shared" ref="AT24:AT32" si="46">AF24+AG24</f>
         <v>52</v>
       </c>
       <c r="AU24" s="2">
-        <f t="shared" ref="AU24:AU32" si="48">AG24+AH24</f>
+        <f t="shared" ref="AU24:AU32" si="47">AG24+AH24</f>
         <v>30</v>
       </c>
       <c r="AV24" s="2">
-        <f t="shared" ref="AV24:AV32" si="49">AH24+AI24</f>
+        <f t="shared" ref="AV24:AV32" si="48">AH24+AI24</f>
         <v>22</v>
       </c>
       <c r="AW24" s="2">
-        <f t="shared" ref="AW24:AW32" si="50">AI24+AJ24</f>
+        <f t="shared" ref="AW24:AW32" si="49">AI24+AJ24</f>
         <v>19</v>
       </c>
       <c r="AX24" s="2"/>
@@ -11026,15 +11183,15 @@
         <v>18</v>
       </c>
       <c r="AZ24">
-        <f t="shared" ref="AZ24:AZ32" si="51">AD24+AF24+AH24+AJ24+AL24+AN24</f>
+        <f t="shared" ref="AZ24:AZ32" si="50">AD24+AF24+AH24+AJ24+AL24+AN24</f>
         <v>101</v>
       </c>
       <c r="BA24">
-        <f t="shared" ref="BA24:BA32" si="52">AE24+AG24+AI24+AK24+AM24+AO24</f>
+        <f t="shared" ref="BA24:BA32" si="51">AE24+AG24+AI24+AK24+AM24+AO24</f>
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="3:55">
+    <row r="25" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>19</v>
       </c>
@@ -11191,27 +11348,27 @@
         <v>19</v>
       </c>
       <c r="AR25" s="2">
+        <f t="shared" ref="AR24:AR32" si="52">AD25+AE25</f>
+        <v>53</v>
+      </c>
+      <c r="AS25" s="2">
         <f t="shared" si="45"/>
-        <v>53</v>
-      </c>
-      <c r="AS25" s="2">
+        <v>40</v>
+      </c>
+      <c r="AT25" s="2">
         <f t="shared" si="46"/>
-        <v>40</v>
-      </c>
-      <c r="AT25" s="2">
+        <v>39</v>
+      </c>
+      <c r="AU25" s="2">
         <f t="shared" si="47"/>
-        <v>39</v>
-      </c>
-      <c r="AU25" s="2">
+        <v>30</v>
+      </c>
+      <c r="AV25" s="2">
         <f t="shared" si="48"/>
-        <v>30</v>
-      </c>
-      <c r="AV25" s="2">
+        <v>23</v>
+      </c>
+      <c r="AW25" s="2">
         <f t="shared" si="49"/>
-        <v>23</v>
-      </c>
-      <c r="AW25" s="2">
-        <f t="shared" si="50"/>
         <v>26</v>
       </c>
       <c r="AX25" s="2"/>
@@ -11219,15 +11376,15 @@
         <v>19</v>
       </c>
       <c r="AZ25">
+        <f t="shared" si="50"/>
+        <v>81</v>
+      </c>
+      <c r="BA25">
         <f t="shared" si="51"/>
-        <v>81</v>
-      </c>
-      <c r="BA25">
-        <f t="shared" si="52"/>
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="3:55">
+    <row r="26" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>20</v>
       </c>
@@ -11384,27 +11541,27 @@
         <v>20</v>
       </c>
       <c r="AR26" s="2">
+        <f t="shared" si="52"/>
+        <v>65</v>
+      </c>
+      <c r="AS26" s="2">
         <f t="shared" si="45"/>
-        <v>65</v>
-      </c>
-      <c r="AS26" s="2">
+        <v>53</v>
+      </c>
+      <c r="AT26" s="2">
         <f t="shared" si="46"/>
-        <v>53</v>
-      </c>
-      <c r="AT26" s="2">
+        <v>33</v>
+      </c>
+      <c r="AU26" s="2">
         <f t="shared" si="47"/>
-        <v>33</v>
-      </c>
-      <c r="AU26" s="2">
+        <v>21</v>
+      </c>
+      <c r="AV26" s="2">
         <f t="shared" si="48"/>
-        <v>21</v>
-      </c>
-      <c r="AV26" s="2">
+        <v>17</v>
+      </c>
+      <c r="AW26" s="2">
         <f t="shared" si="49"/>
-        <v>17</v>
-      </c>
-      <c r="AW26" s="2">
-        <f t="shared" si="50"/>
         <v>12</v>
       </c>
       <c r="AX26" s="2"/>
@@ -11412,15 +11569,15 @@
         <v>20</v>
       </c>
       <c r="AZ26">
+        <f t="shared" si="50"/>
+        <v>89</v>
+      </c>
+      <c r="BA26">
         <f t="shared" si="51"/>
-        <v>89</v>
-      </c>
-      <c r="BA26">
-        <f t="shared" si="52"/>
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="3:55">
+    <row r="27" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>21</v>
       </c>
@@ -11577,27 +11734,27 @@
         <v>21</v>
       </c>
       <c r="AR27" s="2">
+        <f t="shared" si="52"/>
+        <v>43</v>
+      </c>
+      <c r="AS27" s="2">
         <f t="shared" si="45"/>
-        <v>43</v>
-      </c>
-      <c r="AS27" s="2">
+        <v>31</v>
+      </c>
+      <c r="AT27" s="2">
         <f t="shared" si="46"/>
-        <v>31</v>
-      </c>
-      <c r="AT27" s="2">
+        <v>27</v>
+      </c>
+      <c r="AU27" s="2">
         <f t="shared" si="47"/>
-        <v>27</v>
-      </c>
-      <c r="AU27" s="2">
+        <v>28</v>
+      </c>
+      <c r="AV27" s="2">
         <f t="shared" si="48"/>
-        <v>28</v>
-      </c>
-      <c r="AV27" s="2">
+        <v>21</v>
+      </c>
+      <c r="AW27" s="2">
         <f t="shared" si="49"/>
-        <v>21</v>
-      </c>
-      <c r="AW27" s="2">
-        <f t="shared" si="50"/>
         <v>25</v>
       </c>
       <c r="AX27" s="2"/>
@@ -11605,15 +11762,15 @@
         <v>21</v>
       </c>
       <c r="AZ27">
+        <f t="shared" si="50"/>
+        <v>74</v>
+      </c>
+      <c r="BA27">
         <f t="shared" si="51"/>
-        <v>74</v>
-      </c>
-      <c r="BA27">
-        <f t="shared" si="52"/>
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="3:55">
+    <row r="28" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>22</v>
       </c>
@@ -11770,27 +11927,27 @@
         <v>22</v>
       </c>
       <c r="AR28" s="2">
+        <f t="shared" si="52"/>
+        <v>60</v>
+      </c>
+      <c r="AS28" s="2">
         <f t="shared" si="45"/>
-        <v>60</v>
-      </c>
-      <c r="AS28" s="2">
+        <v>57</v>
+      </c>
+      <c r="AT28" s="2">
         <f t="shared" si="46"/>
-        <v>57</v>
-      </c>
-      <c r="AT28" s="2">
+        <v>46</v>
+      </c>
+      <c r="AU28" s="2">
         <f t="shared" si="47"/>
-        <v>46</v>
-      </c>
-      <c r="AU28" s="2">
+        <v>37</v>
+      </c>
+      <c r="AV28" s="2">
         <f t="shared" si="48"/>
-        <v>37</v>
-      </c>
-      <c r="AV28" s="2">
+        <v>27</v>
+      </c>
+      <c r="AW28" s="2">
         <f t="shared" si="49"/>
-        <v>27</v>
-      </c>
-      <c r="AW28" s="2">
-        <f t="shared" si="50"/>
         <v>26</v>
       </c>
       <c r="AX28" s="2"/>
@@ -11798,15 +11955,15 @@
         <v>22</v>
       </c>
       <c r="AZ28">
+        <f t="shared" si="50"/>
+        <v>102</v>
+      </c>
+      <c r="BA28">
         <f t="shared" si="51"/>
-        <v>102</v>
-      </c>
-      <c r="BA28">
-        <f t="shared" si="52"/>
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="3:55">
+    <row r="29" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>23</v>
       </c>
@@ -11961,42 +12118,42 @@
         <v>23</v>
       </c>
       <c r="AR29" s="2">
+        <f t="shared" si="52"/>
+        <v>46</v>
+      </c>
+      <c r="AS29" s="2">
         <f t="shared" si="45"/>
         <v>46</v>
       </c>
-      <c r="AS29" s="2">
+      <c r="AT29" s="2">
         <f t="shared" si="46"/>
-        <v>46</v>
-      </c>
-      <c r="AT29" s="2">
+        <v>35</v>
+      </c>
+      <c r="AU29" s="2">
         <f t="shared" si="47"/>
-        <v>35</v>
-      </c>
-      <c r="AU29" s="2">
+        <v>23</v>
+      </c>
+      <c r="AV29" s="2">
         <f t="shared" si="48"/>
-        <v>23</v>
-      </c>
-      <c r="AV29" s="2">
+        <v>11</v>
+      </c>
+      <c r="AW29" s="2">
         <f t="shared" si="49"/>
-        <v>11</v>
-      </c>
-      <c r="AW29" s="2">
-        <f t="shared" si="50"/>
         <v>13</v>
       </c>
       <c r="AY29" t="s">
         <v>23</v>
       </c>
       <c r="AZ29">
+        <f t="shared" si="50"/>
+        <v>78</v>
+      </c>
+      <c r="BA29">
         <f t="shared" si="51"/>
-        <v>78</v>
-      </c>
-      <c r="BA29">
-        <f t="shared" si="52"/>
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="3:55">
+    <row r="30" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>24</v>
       </c>
@@ -12151,42 +12308,42 @@
         <v>24</v>
       </c>
       <c r="AR30" s="2">
+        <f t="shared" si="52"/>
+        <v>62</v>
+      </c>
+      <c r="AS30" s="2">
         <f t="shared" si="45"/>
-        <v>62</v>
-      </c>
-      <c r="AS30" s="2">
+        <v>43</v>
+      </c>
+      <c r="AT30" s="2">
         <f t="shared" si="46"/>
-        <v>43</v>
-      </c>
-      <c r="AT30" s="2">
+        <v>24</v>
+      </c>
+      <c r="AU30" s="2">
         <f t="shared" si="47"/>
-        <v>24</v>
-      </c>
-      <c r="AU30" s="2">
+        <v>14</v>
+      </c>
+      <c r="AV30" s="2">
         <f t="shared" si="48"/>
         <v>14</v>
       </c>
-      <c r="AV30" s="2">
+      <c r="AW30" s="2">
         <f t="shared" si="49"/>
-        <v>14</v>
-      </c>
-      <c r="AW30" s="2">
-        <f t="shared" si="50"/>
         <v>22</v>
       </c>
       <c r="AY30" t="s">
         <v>24</v>
       </c>
       <c r="AZ30">
+        <f t="shared" si="50"/>
+        <v>89</v>
+      </c>
+      <c r="BA30">
         <f t="shared" si="51"/>
-        <v>89</v>
-      </c>
-      <c r="BA30">
-        <f t="shared" si="52"/>
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="3:55">
+    <row r="31" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>25</v>
       </c>
@@ -12341,42 +12498,42 @@
         <v>25</v>
       </c>
       <c r="AR31" s="2">
+        <f t="shared" si="52"/>
+        <v>53</v>
+      </c>
+      <c r="AS31" s="2">
         <f t="shared" si="45"/>
-        <v>53</v>
-      </c>
-      <c r="AS31" s="2">
+        <v>42</v>
+      </c>
+      <c r="AT31" s="2">
         <f t="shared" si="46"/>
-        <v>42</v>
-      </c>
-      <c r="AT31" s="2">
+        <v>41</v>
+      </c>
+      <c r="AU31" s="2">
         <f t="shared" si="47"/>
-        <v>41</v>
-      </c>
-      <c r="AU31" s="2">
+        <v>37</v>
+      </c>
+      <c r="AV31" s="2">
         <f t="shared" si="48"/>
-        <v>37</v>
-      </c>
-      <c r="AV31" s="2">
+        <v>25</v>
+      </c>
+      <c r="AW31" s="2">
         <f t="shared" si="49"/>
-        <v>25</v>
-      </c>
-      <c r="AW31" s="2">
-        <f t="shared" si="50"/>
         <v>31</v>
       </c>
       <c r="AY31" t="s">
         <v>25</v>
       </c>
       <c r="AZ31">
+        <f t="shared" si="50"/>
+        <v>88</v>
+      </c>
+      <c r="BA31">
         <f t="shared" si="51"/>
-        <v>88</v>
-      </c>
-      <c r="BA31">
-        <f t="shared" si="52"/>
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="3:55">
+    <row r="32" spans="3:55" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>26</v>
       </c>
@@ -12531,42 +12688,42 @@
         <v>26</v>
       </c>
       <c r="AR32" s="2">
+        <f t="shared" si="52"/>
+        <v>69</v>
+      </c>
+      <c r="AS32" s="2">
         <f t="shared" si="45"/>
-        <v>69</v>
-      </c>
-      <c r="AS32" s="2">
+        <v>57</v>
+      </c>
+      <c r="AT32" s="2">
         <f t="shared" si="46"/>
-        <v>57</v>
-      </c>
-      <c r="AT32" s="2">
+        <v>42</v>
+      </c>
+      <c r="AU32" s="2">
         <f t="shared" si="47"/>
-        <v>42</v>
-      </c>
-      <c r="AU32" s="2">
+        <v>23</v>
+      </c>
+      <c r="AV32" s="2">
         <f t="shared" si="48"/>
-        <v>23</v>
-      </c>
-      <c r="AV32" s="2">
+        <v>12</v>
+      </c>
+      <c r="AW32" s="2">
         <f t="shared" si="49"/>
-        <v>12</v>
-      </c>
-      <c r="AW32" s="2">
-        <f t="shared" si="50"/>
         <v>13</v>
       </c>
       <c r="AY32" t="s">
         <v>26</v>
       </c>
       <c r="AZ32">
+        <f t="shared" si="50"/>
+        <v>91</v>
+      </c>
+      <c r="BA32">
         <f t="shared" si="51"/>
-        <v>91</v>
-      </c>
-      <c r="BA32">
-        <f t="shared" si="52"/>
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="43:49">
+    <row r="35" spans="43:49" x14ac:dyDescent="0.25">
       <c r="AR35" t="s">
         <v>39</v>
       </c>
@@ -12586,7 +12743,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="43:49">
+    <row r="36" spans="43:49" x14ac:dyDescent="0.25">
       <c r="AQ36" t="s">
         <v>17</v>
       </c>
@@ -12609,7 +12766,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="43:49">
+    <row r="37" spans="43:49" x14ac:dyDescent="0.25">
       <c r="AQ37" t="s">
         <v>18</v>
       </c>
@@ -12632,7 +12789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="43:49">
+    <row r="38" spans="43:49" x14ac:dyDescent="0.25">
       <c r="AQ38" t="s">
         <v>19</v>
       </c>
@@ -12655,7 +12812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="43:49">
+    <row r="39" spans="43:49" x14ac:dyDescent="0.25">
       <c r="AQ39" t="s">
         <v>20</v>
       </c>
@@ -12678,7 +12835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="43:49">
+    <row r="40" spans="43:49" x14ac:dyDescent="0.25">
       <c r="AQ40" t="s">
         <v>21</v>
       </c>
@@ -12701,7 +12858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="43:49">
+    <row r="41" spans="43:49" x14ac:dyDescent="0.25">
       <c r="AQ41" t="s">
         <v>22</v>
       </c>
@@ -12724,7 +12881,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="43:49">
+    <row r="42" spans="43:49" x14ac:dyDescent="0.25">
       <c r="AQ42" t="s">
         <v>23</v>
       </c>
@@ -12747,7 +12904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="43:49">
+    <row r="43" spans="43:49" x14ac:dyDescent="0.25">
       <c r="AQ43" t="s">
         <v>24</v>
       </c>
@@ -12770,7 +12927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="43:49">
+    <row r="44" spans="43:49" x14ac:dyDescent="0.25">
       <c r="AQ44" t="s">
         <v>25</v>
       </c>
@@ -12793,7 +12950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="43:49">
+    <row r="45" spans="43:49" x14ac:dyDescent="0.25">
       <c r="AQ45" t="s">
         <v>26</v>
       </c>
@@ -12816,24 +12973,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="5:17">
-      <c r="E83" s="21" t="s">
+    <row r="83" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E83" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="F83" s="21"/>
-      <c r="G83" s="21"/>
-      <c r="H83" s="21"/>
-      <c r="I83" s="21"/>
-      <c r="J83" s="21"/>
-      <c r="K83" s="21"/>
-      <c r="L83" s="21"/>
-      <c r="M83" s="21"/>
-      <c r="N83" s="21"/>
-      <c r="O83" s="21"/>
-      <c r="P83" s="21"/>
-      <c r="Q83" s="21"/>
+      <c r="F83" s="30"/>
+      <c r="G83" s="30"/>
+      <c r="H83" s="30"/>
+      <c r="I83" s="30"/>
+      <c r="J83" s="30"/>
+      <c r="K83" s="30"/>
+      <c r="L83" s="30"/>
+      <c r="M83" s="30"/>
+      <c r="N83" s="30"/>
+      <c r="O83" s="30"/>
+      <c r="P83" s="30"/>
+      <c r="Q83" s="30"/>
     </row>
-    <row r="84" spans="5:17">
+    <row r="84" spans="5:17" x14ac:dyDescent="0.25">
       <c r="F84">
         <v>1</v>
       </c>
@@ -12871,7 +13028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="5:17">
+    <row r="85" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E85" t="s">
         <v>45</v>
       </c>
@@ -12914,12 +13071,48 @@
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="X4:AA4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="T4:W4"/>
+    <mergeCell ref="E83:Q83"/>
+    <mergeCell ref="AN21:AO21"/>
+    <mergeCell ref="T20:W20"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="X20:AA20"/>
+    <mergeCell ref="X21:Y21"/>
+    <mergeCell ref="Z21:AA21"/>
+    <mergeCell ref="AD21:AE21"/>
+    <mergeCell ref="AF21:AG21"/>
+    <mergeCell ref="AH21:AI21"/>
+    <mergeCell ref="AJ21:AK21"/>
+    <mergeCell ref="AL21:AM21"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P20:S20"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="AT5:AU5"/>
+    <mergeCell ref="AV5:AW5"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AL5:AM5"/>
+    <mergeCell ref="AN5:AO5"/>
+    <mergeCell ref="AP5:AQ5"/>
+    <mergeCell ref="AX5:AY5"/>
+    <mergeCell ref="AZ5:BA5"/>
+    <mergeCell ref="BB5:BC5"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="AR5:AS5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AF5:AG5"/>
     <mergeCell ref="AZ4:BC4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
@@ -12936,48 +13129,12 @@
     <mergeCell ref="AN4:AQ4"/>
     <mergeCell ref="AR4:AU4"/>
     <mergeCell ref="AV4:AY4"/>
-    <mergeCell ref="AX5:AY5"/>
-    <mergeCell ref="AZ5:BA5"/>
-    <mergeCell ref="BB5:BC5"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="AR5:AS5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="P20:S20"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="AT5:AU5"/>
-    <mergeCell ref="AV5:AW5"/>
-    <mergeCell ref="AH5:AI5"/>
-    <mergeCell ref="AJ5:AK5"/>
-    <mergeCell ref="AL5:AM5"/>
-    <mergeCell ref="AN5:AO5"/>
-    <mergeCell ref="AP5:AQ5"/>
-    <mergeCell ref="E83:Q83"/>
-    <mergeCell ref="AN21:AO21"/>
-    <mergeCell ref="T20:W20"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="X20:AA20"/>
-    <mergeCell ref="X21:Y21"/>
-    <mergeCell ref="Z21:AA21"/>
-    <mergeCell ref="AD21:AE21"/>
-    <mergeCell ref="AF21:AG21"/>
-    <mergeCell ref="AH21:AI21"/>
-    <mergeCell ref="AJ21:AK21"/>
-    <mergeCell ref="AL21:AM21"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="X4:AA4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="T4:W4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12986,186 +13143,186 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="39" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="39" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="39">
+      <c r="B3" s="21">
         <v>5213100129</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="21">
         <v>5213100140</v>
       </c>
-      <c r="D3" s="39">
+      <c r="D3" s="21">
         <v>5212100084</v>
       </c>
-      <c r="E3" s="39"/>
+      <c r="E3" s="21"/>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="39" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="39" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="21">
         <v>5213100193</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="21">
         <v>5213100154</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="21">
         <v>5213100100</v>
       </c>
-      <c r="E7" s="39"/>
+      <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="39"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="39" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="39" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="39" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="39">
+      <c r="B12" s="21">
         <v>5213100180</v>
       </c>
-      <c r="C12" s="39">
+      <c r="C12" s="21">
         <v>5213100179</v>
       </c>
-      <c r="D12" s="39">
+      <c r="D12" s="21">
         <v>5213100139</v>
       </c>
-      <c r="E12" s="39">
+      <c r="E12" s="21">
         <v>5213100117</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="39"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="39" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="39" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="39" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="39">
+      <c r="B17" s="21">
         <v>5212100001</v>
       </c>
-      <c r="C17" s="39">
+      <c r="C17" s="21">
         <v>5213100039</v>
       </c>
-      <c r="D17" s="39">
+      <c r="D17" s="21">
         <v>5213100101</v>
       </c>
-      <c r="E17" s="39">
+      <c r="E17" s="21">
         <v>5213100028</v>
       </c>
     </row>

</xml_diff>